<commit_message>
Um please just save this updated excel
</commit_message>
<xml_diff>
--- a/messy-project-directory/data/Survey_Data.xlsx
+++ b/messy-project-directory/data/Survey_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cassidy/Documents/tfcb-homework02/messy-project-directory/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AA3562-229A-7F42-9A19-C407DEBA698E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EBBF14-4CFE-B34B-BEE0-2FCFCC42602A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1980" yWindow="1400" windowWidth="25120" windowHeight="15580" tabRatio="481" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,7 +85,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -159,16 +159,16 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -561,7 +561,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -605,7 +605,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">

</xml_diff>